<commit_message>
added new case in test
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myfw\newsoul-selenium-framework\newsoul-selenium-framework\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="150" windowWidth="18195" windowHeight="8475"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="107">
   <si>
     <t>ID</t>
   </si>
@@ -403,6 +408,12 @@
   </si>
   <si>
     <t>Фильтра сбросил все свои значения. Данные на странице отображаются как при первой загрузке</t>
+  </si>
+  <si>
+    <t>выполнение</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -468,7 +479,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -476,14 +487,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -521,9 +535,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,7 +572,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,7 +607,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -770,8 +784,8 @@
   <dimension ref="A1:AC239"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,6 +795,7 @@
     <col min="4" max="4" width="37.28515625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
     <col min="6" max="6" width="35.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
@@ -802,7 +817,9 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -841,7 +858,9 @@
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -877,7 +896,9 @@
       <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>

</xml_diff>